<commit_message>
The report is finished. All calculations are in the excel file and matlab files. We added bom pdf and other pdfs as well. Project is finished!
</commit_message>
<xml_diff>
--- a/EE464_design.xlsx
+++ b/EE464_design.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Emre Deniz\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F1C2274-CB4F-4666-8105-131D570DC893}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DEAAA3A-1BC7-42B5-A711-BC7C05D794E0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{EA313EEF-6F9F-46E5-9606-4FB4CEBF9422}"/>
+    <workbookView xWindow="2970" yWindow="1380" windowWidth="25320" windowHeight="12000" xr2:uid="{EA313EEF-6F9F-46E5-9606-4FB4CEBF9422}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
   <si>
     <t>Vin</t>
   </si>
@@ -126,13 +126,55 @@
   </si>
   <si>
     <t>https://www.mag-inc.com/Media/Magnetics/Datasheets/0R43515EC.pdf</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>Length</t>
+  </si>
+  <si>
+    <t>R1</t>
+  </si>
+  <si>
+    <t>Res/m</t>
+  </si>
+  <si>
+    <t>R2</t>
+  </si>
+  <si>
+    <t>R3</t>
+  </si>
+  <si>
+    <t>D1 ideal</t>
+  </si>
+  <si>
+    <t>D2 ideal</t>
+  </si>
+  <si>
+    <t>D1 NON</t>
+  </si>
+  <si>
+    <t>D2 NON</t>
+  </si>
+  <si>
+    <t>Compansator</t>
+  </si>
+  <si>
+    <t>f_lc</t>
+  </si>
+  <si>
+    <t>f_esr</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -147,6 +189,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF202122"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -170,10 +218,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -489,10 +538,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8CA113AD-EA5B-4797-B327-9D0EC0E22A4C}">
-  <dimension ref="C3:R23"/>
+  <dimension ref="C3:R34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R26" sqref="R26"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -660,7 +709,7 @@
       </c>
       <c r="R12" s="1">
         <f>O12*K7*H13</f>
-        <v>32.373000000000005</v>
+        <v>43.164000000000001</v>
       </c>
     </row>
     <row r="13" spans="3:18" x14ac:dyDescent="0.25">
@@ -668,12 +717,12 @@
         <v>8</v>
       </c>
       <c r="G13" s="1">
-        <f>1.5*G9</f>
-        <v>33.103448275862071</v>
+        <f>2*G9</f>
+        <v>44.137931034482762</v>
       </c>
       <c r="H13" s="1">
         <f>ROUND(G13,0)</f>
-        <v>33</v>
+        <v>44</v>
       </c>
       <c r="Q13" t="s">
         <v>24</v>
@@ -693,7 +742,7 @@
       </c>
       <c r="R14" s="1">
         <f>SUM(R13+R12+R11)</f>
-        <v>61.149000000000001</v>
+        <v>71.94</v>
       </c>
     </row>
     <row r="15" spans="3:18" x14ac:dyDescent="0.25">
@@ -705,7 +754,15 @@
         <v>2.667E-6</v>
       </c>
     </row>
-    <row r="17" spans="6:18" x14ac:dyDescent="0.25">
+    <row r="16" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="M16" t="s">
+        <v>35</v>
+      </c>
+      <c r="N16" s="3">
+        <v>52.96</v>
+      </c>
+    </row>
+    <row r="17" spans="3:18" x14ac:dyDescent="0.25">
       <c r="F17" t="s">
         <v>14</v>
       </c>
@@ -714,7 +771,19 @@
         <v>1.2989336504161714E-3</v>
       </c>
     </row>
-    <row r="18" spans="6:18" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="C18" t="s">
+        <v>38</v>
+      </c>
+      <c r="D18">
+        <v>15.65</v>
+      </c>
+      <c r="M18" t="s">
+        <v>31</v>
+      </c>
+      <c r="N18">
+        <v>9.3000000000000007</v>
+      </c>
       <c r="Q18" t="s">
         <v>25</v>
       </c>
@@ -722,7 +791,19 @@
         <v>9.8000000000000007</v>
       </c>
     </row>
-    <row r="19" spans="6:18" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="C19" t="s">
+        <v>39</v>
+      </c>
+      <c r="D19">
+        <v>31.25</v>
+      </c>
+      <c r="M19" t="s">
+        <v>32</v>
+      </c>
+      <c r="N19">
+        <v>8</v>
+      </c>
       <c r="Q19" t="s">
         <v>26</v>
       </c>
@@ -730,7 +811,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="20" spans="6:18" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:18" x14ac:dyDescent="0.25">
       <c r="F20" t="s">
         <v>18</v>
       </c>
@@ -739,7 +820,7 @@
         <v>0.23537190215872694</v>
       </c>
     </row>
-    <row r="21" spans="6:18" x14ac:dyDescent="0.25">
+    <row r="21" spans="3:18" x14ac:dyDescent="0.25">
       <c r="Q21" t="s">
         <v>27</v>
       </c>
@@ -748,13 +829,82 @@
         <v>156.80000000000001</v>
       </c>
     </row>
-    <row r="23" spans="6:18" x14ac:dyDescent="0.25">
+    <row r="23" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="M23" t="s">
+        <v>33</v>
+      </c>
+      <c r="N23">
+        <f>2*PI()*(N19+N18)/2</f>
+        <v>54.349552907103423</v>
+      </c>
       <c r="Q23" t="s">
         <v>28</v>
       </c>
       <c r="R23" s="1">
         <f>R14/R21</f>
-        <v>0.38998086734693876</v>
+        <v>0.45880102040816323</v>
+      </c>
+    </row>
+    <row r="24" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="C24" t="s">
+        <v>40</v>
+      </c>
+      <c r="D24">
+        <v>43.5</v>
+      </c>
+    </row>
+    <row r="25" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="C25" t="s">
+        <v>41</v>
+      </c>
+      <c r="D25">
+        <v>22.05</v>
+      </c>
+      <c r="M25" t="s">
+        <v>34</v>
+      </c>
+      <c r="N25" s="1">
+        <f>N23*H9*N16/1000/2</f>
+        <v>31.661875541562168</v>
+      </c>
+    </row>
+    <row r="26" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="M26" t="s">
+        <v>36</v>
+      </c>
+      <c r="N26" s="1">
+        <f>N23*N16*H13/1000/3</f>
+        <v>42.215834055416231</v>
+      </c>
+    </row>
+    <row r="27" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="M27" t="s">
+        <v>37</v>
+      </c>
+      <c r="N27" s="1">
+        <f>N25</f>
+        <v>31.661875541562168</v>
+      </c>
+    </row>
+    <row r="31" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="D31" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="33" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D33" t="s">
+        <v>43</v>
+      </c>
+      <c r="E33" s="1">
+        <v>1110</v>
+      </c>
+    </row>
+    <row r="34" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D34" t="s">
+        <v>44</v>
+      </c>
+      <c r="E34" s="1">
+        <v>1760000</v>
       </c>
     </row>
   </sheetData>
@@ -762,5 +912,6 @@
     <hyperlink ref="N4" r:id="rId1" xr:uid="{AF1DB343-0529-4431-A535-498A5AA69963}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>